<commit_message>
cool changes for baris form editable now
</commit_message>
<xml_diff>
--- a/lolMineSite/results/api/lol.xlsx
+++ b/lolMineSite/results/api/lol.xlsx
@@ -468,7 +468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1528,34 +1528,32 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>8.743415893791914</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
-        <v>18485.6</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>0.04002778947189373</v>
+        <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>229.6</v>
-      </c>
-      <c r="G31" t="s">
-        <v>10</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G31" t="s"/>
       <c r="H31" t="s">
         <v>11</v>
       </c>
       <c r="I31" t="n">
-        <v>0.1242981404229443</v>
+        <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>0.00490817992779415</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1563,34 +1561,34 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>1.516374128646075</v>
+        <v>1.297897196261682</v>
       </c>
       <c r="C32" t="n">
-        <v>2265</v>
+        <v>2222</v>
       </c>
       <c r="D32" t="n">
-        <v>0.007052291106241539</v>
+        <v>0.002628504672897196</v>
       </c>
       <c r="E32" t="n">
-        <v>11</v>
+        <v>4.5</v>
       </c>
       <c r="F32" t="n">
-        <v>147.4</v>
+        <v>272.5</v>
       </c>
       <c r="G32" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="H32" t="s">
         <v>11</v>
       </c>
       <c r="I32" t="n">
-        <v>0.1023365636679312</v>
+        <v>0.1591705607476636</v>
       </c>
       <c r="J32" t="n">
-        <v>10</v>
+        <v>23.5</v>
       </c>
       <c r="K32" t="n">
-        <v>0.006562597733466744</v>
+        <v>0.01372663551401869</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1598,104 +1596,65 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>3.47305785123967</v>
+        <v>0</v>
       </c>
       <c r="C33" t="n">
-        <v>6303.6</v>
+        <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>0.01641873278236915</v>
+        <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>29.8</v>
+        <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>48.2</v>
-      </c>
-      <c r="G33" t="s">
-        <v>13</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G33" t="s"/>
       <c r="H33" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I33" t="n">
-        <v>0.0265564738292011</v>
+        <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>3.2</v>
+        <v>0</v>
       </c>
       <c r="K33" t="n">
-        <v>0.001763085399449036</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="1" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>9.941856090662251</v>
+        <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>18698.8</v>
+        <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>0.04483485832705165</v>
+        <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>89.2</v>
+        <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>387</v>
-      </c>
-      <c r="G34" t="s">
-        <v>14</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G34" t="s"/>
       <c r="H34" t="s">
         <v>11</v>
       </c>
       <c r="I34" t="n">
-        <v>0.2388622264459989</v>
+        <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>18.2</v>
+        <v>0</v>
       </c>
       <c r="K34" t="n">
-        <v>0.01057342292541073</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="n">
-        <v>2.739134966128192</v>
-      </c>
-      <c r="C35" t="n">
-        <v>5256.4</v>
-      </c>
-      <c r="D35" t="n">
-        <v>0.02136529442417926</v>
-      </c>
-      <c r="E35" t="n">
-        <v>41</v>
-      </c>
-      <c r="F35" t="n">
-        <v>166.6</v>
-      </c>
-      <c r="G35" t="s">
-        <v>24</v>
-      </c>
-      <c r="H35" t="s">
-        <v>25</v>
-      </c>
-      <c r="I35" t="n">
-        <v>0.08681605002605523</v>
-      </c>
-      <c r="J35" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="K35" t="n">
-        <v>0.00198019801980198</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AHP implied to system
</commit_message>
<xml_diff>
--- a/lolMineSite/results/api/lol.xlsx
+++ b/lolMineSite/results/api/lol.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
   <si>
     <t>Aggression Point</t>
   </si>
@@ -141,6 +141,21 @@
   </si>
   <si>
     <t>PYKEntakill</t>
+  </si>
+  <si>
+    <t>JaIisco</t>
+  </si>
+  <si>
+    <t>Booogeyman</t>
+  </si>
+  <si>
+    <t>Cantare</t>
+  </si>
+  <si>
+    <t>Poppy Gods</t>
+  </si>
+  <si>
+    <t>Ithryn L</t>
   </si>
 </sst>
 </file>
@@ -489,7 +504,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:K81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2343,22 +2358,22 @@
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="1" t="n">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>8.743415893791914</v>
+        <v>3.203383214053351</v>
       </c>
       <c r="C54" t="n">
-        <v>18485.6</v>
+        <v>4923.6</v>
       </c>
       <c r="D54" t="n">
-        <v>0.04002778947189373</v>
+        <v>0.01535458685751464</v>
       </c>
       <c r="E54" t="n">
-        <v>84</v>
+        <v>23.6</v>
       </c>
       <c r="F54" t="n">
-        <v>229.6</v>
+        <v>126</v>
       </c>
       <c r="G54" t="s">
         <v>10</v>
@@ -2367,33 +2382,33 @@
         <v>11</v>
       </c>
       <c r="I54" t="n">
-        <v>0.1242981404229443</v>
+        <v>0.08197787898503578</v>
       </c>
       <c r="J54" t="n">
-        <v>10</v>
+        <v>3.4</v>
       </c>
       <c r="K54" t="n">
-        <v>0.00490817992779415</v>
+        <v>0.0022121014964216</v>
       </c>
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="1" t="n">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>2.732152492161565</v>
+        <v>1.775319622012229</v>
       </c>
       <c r="C55" t="n">
-        <v>4754.8</v>
+        <v>3193.8</v>
       </c>
       <c r="D55" t="n">
-        <v>0.01058489950476475</v>
+        <v>0.01634241245136187</v>
       </c>
       <c r="E55" t="n">
-        <v>18.2</v>
+        <v>29.4</v>
       </c>
       <c r="F55" t="n">
-        <v>286.2</v>
+        <v>41</v>
       </c>
       <c r="G55" t="s">
         <v>12</v>
@@ -2402,33 +2417,33 @@
         <v>11</v>
       </c>
       <c r="I55" t="n">
-        <v>0.1699525553653752</v>
+        <v>0.02279043913285158</v>
       </c>
       <c r="J55" t="n">
-        <v>21.2</v>
+        <v>4.4</v>
       </c>
       <c r="K55" t="n">
-        <v>0.01215288164343084</v>
+        <v>0.002445803224013341</v>
       </c>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" s="1" t="n">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>3.151435406698565</v>
+        <v>4.58653314427508</v>
       </c>
       <c r="C56" t="n">
-        <v>5269.2</v>
+        <v>8017.8</v>
       </c>
       <c r="D56" t="n">
-        <v>0.02009569377990431</v>
+        <v>0.03247285569866215</v>
       </c>
       <c r="E56" t="n">
-        <v>33.6</v>
+        <v>56.2</v>
       </c>
       <c r="F56" t="n">
-        <v>116</v>
+        <v>187.4</v>
       </c>
       <c r="G56" t="s">
         <v>13</v>
@@ -2437,33 +2452,33 @@
         <v>11</v>
       </c>
       <c r="I56" t="n">
-        <v>0.06937799043062201</v>
+        <v>0.1066721808657292</v>
       </c>
       <c r="J56" t="n">
-        <v>2.6</v>
+        <v>5.4</v>
       </c>
       <c r="K56" t="n">
-        <v>0.001555023923444976</v>
+        <v>0.003094384707287933</v>
       </c>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="1" t="n">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>6.383743300662566</v>
+        <v>3.650427670597207</v>
       </c>
       <c r="C57" t="n">
-        <v>12258.8</v>
+        <v>5630</v>
       </c>
       <c r="D57" t="n">
-        <v>0.04023672888935409</v>
+        <v>0.02674180615384204</v>
       </c>
       <c r="E57" t="n">
-        <v>81</v>
+        <v>44.4</v>
       </c>
       <c r="F57" t="n">
-        <v>253.6</v>
+        <v>227.4</v>
       </c>
       <c r="G57" t="s">
         <v>14</v>
@@ -2472,47 +2487,852 @@
         <v>11</v>
       </c>
       <c r="I57" t="n">
-        <v>0.13711238076999</v>
+        <v>0.1559623334516667</v>
       </c>
       <c r="J57" t="n">
-        <v>14.8</v>
+        <v>11.4</v>
       </c>
       <c r="K57" t="n">
-        <v>0.007707535390238893</v>
+        <v>0.00728984276207101</v>
       </c>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>1.657101658255227</v>
+      </c>
+      <c r="C58" t="n">
+        <v>2298.4</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.02033165104542177</v>
+      </c>
+      <c r="E58" t="n">
+        <v>28.2</v>
+      </c>
+      <c r="F58" t="n">
+        <v>69.2</v>
+      </c>
+      <c r="G58" t="s">
+        <v>24</v>
+      </c>
+      <c r="H58" t="s">
+        <v>25</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0.04989185291997116</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0.0001441961067051189</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>2.219149527515286</v>
+      </c>
+      <c r="C59" t="n">
+        <v>3992.25</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.02042801556420233</v>
+      </c>
+      <c r="E59" t="n">
+        <v>36.75</v>
+      </c>
+      <c r="F59" t="n">
+        <v>51.25</v>
+      </c>
+      <c r="G59" t="s">
+        <v>12</v>
+      </c>
+      <c r="H59" t="s">
+        <v>11</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.02848804891606448</v>
+      </c>
+      <c r="J59" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0.003057254030016676</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>5.73316643034385</v>
+      </c>
+      <c r="C60" t="n">
+        <v>10022.25</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.04059106962332769</v>
+      </c>
+      <c r="E60" t="n">
+        <v>70.25</v>
+      </c>
+      <c r="F60" t="n">
+        <v>234.25</v>
+      </c>
+      <c r="G60" t="s">
+        <v>13</v>
+      </c>
+      <c r="H60" t="s">
+        <v>11</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0.1333402260821616</v>
+      </c>
+      <c r="J60" t="n">
+        <v>6.75</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0.003867980884109916</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>2.071377072819034</v>
+      </c>
+      <c r="C61" t="n">
+        <v>2873</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.02541456380677722</v>
+      </c>
+      <c r="E61" t="n">
+        <v>35.25</v>
+      </c>
+      <c r="F61" t="n">
+        <v>86.5</v>
+      </c>
+      <c r="G61" t="s">
+        <v>24</v>
+      </c>
+      <c r="H61" t="s">
+        <v>25</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0.06236481614996395</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0.0001802451333813987</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>6.451745292628223</v>
+      </c>
+      <c r="C62" t="n">
+        <v>11335.4</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.03638221087160513</v>
+      </c>
+      <c r="E62" t="n">
+        <v>65.8</v>
+      </c>
+      <c r="F62" t="n">
+        <v>293</v>
+      </c>
+      <c r="G62" t="s">
+        <v>14</v>
+      </c>
+      <c r="H62" t="s">
+        <v>11</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.1866635435052542</v>
+      </c>
+      <c r="J62" t="n">
+        <v>13.6</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0.008109015746182139</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="B58" t="n">
+      <c r="B63" t="n">
+        <v>4.768732242866904</v>
+      </c>
+      <c r="C63" t="n">
+        <v>7445</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.03195378050521529</v>
+      </c>
+      <c r="E63" t="n">
+        <v>50.16666666666666</v>
+      </c>
+      <c r="F63" t="n">
+        <v>190.1666666666667</v>
+      </c>
+      <c r="G63" t="s">
+        <v>10</v>
+      </c>
+      <c r="H63" t="s">
+        <v>11</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.1218115490704444</v>
+      </c>
+      <c r="J63" t="n">
+        <v>4.833333333333333</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0.003099699320719843</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>1.479433018343524</v>
+      </c>
+      <c r="C64" t="n">
+        <v>2661.5</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.01361867704280156</v>
+      </c>
+      <c r="E64" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="F64" t="n">
+        <v>34.16666666666666</v>
+      </c>
+      <c r="G64" t="s">
+        <v>12</v>
+      </c>
+      <c r="H64" t="s">
+        <v>11</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0.01899203261070965</v>
+      </c>
+      <c r="J64" t="n">
+        <v>3.666666666666667</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0.002038169353344451</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>3.822110953562567</v>
+      </c>
+      <c r="C65" t="n">
+        <v>6681.5</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.02706071308221846</v>
+      </c>
+      <c r="E65" t="n">
+        <v>46.83333333333334</v>
+      </c>
+      <c r="F65" t="n">
+        <v>156.1666666666667</v>
+      </c>
+      <c r="G65" t="s">
+        <v>13</v>
+      </c>
+      <c r="H65" t="s">
+        <v>11</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0.08889348405477437</v>
+      </c>
+      <c r="J65" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="K65" t="n">
+        <v>0.002578653922739944</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>7.109574936737488</v>
+      </c>
+      <c r="C66" t="n">
+        <v>12432.33333333333</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.0492776887849563</v>
+      </c>
+      <c r="E66" t="n">
+        <v>87.5</v>
+      </c>
+      <c r="F66" t="n">
+        <v>326.8333333333333</v>
+      </c>
+      <c r="G66" t="s">
+        <v>14</v>
+      </c>
+      <c r="H66" t="s">
+        <v>11</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0.2035312852870734</v>
+      </c>
+      <c r="J66" t="n">
+        <v>17.83333333333333</v>
+      </c>
+      <c r="K66" t="n">
+        <v>0.01053000296511503</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>5.251755500694689</v>
+      </c>
+      <c r="C67" t="n">
+        <v>9529.166666666666</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.06558663539837613</v>
+      </c>
+      <c r="E67" t="n">
+        <v>113.5</v>
+      </c>
+      <c r="F67" t="n">
+        <v>266.6666666666667</v>
+      </c>
+      <c r="G67" t="s">
+        <v>42</v>
+      </c>
+      <c r="H67" t="s">
+        <v>11</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0.1534088627803535</v>
+      </c>
+      <c r="J67" t="n">
+        <v>8.333333333333334</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0.004630813408796165</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>3.393041794365421</v>
+      </c>
+      <c r="C68" t="n">
+        <v>4321.833333333333</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.03561639816772885</v>
+      </c>
+      <c r="E68" t="n">
+        <v>45.83333333333334</v>
+      </c>
+      <c r="F68" t="n">
+        <v>98</v>
+      </c>
+      <c r="G68" t="s">
+        <v>24</v>
+      </c>
+      <c r="H68" t="s">
+        <v>25</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0.0753000669539336</v>
+      </c>
+      <c r="J68" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K68" t="n">
+        <v>0.001234990624037989</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>1.548397645519948</v>
+      </c>
+      <c r="C69" t="n">
+        <v>2367.5</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.02043819489862655</v>
+      </c>
+      <c r="E69" t="n">
+        <v>31.25</v>
+      </c>
+      <c r="F69" t="n">
+        <v>97.5</v>
+      </c>
+      <c r="G69" t="s">
+        <v>43</v>
+      </c>
+      <c r="H69" t="s">
+        <v>18</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0.06376716808371484</v>
+      </c>
+      <c r="J69" t="n">
+        <v>4</v>
+      </c>
+      <c r="K69" t="n">
+        <v>0.002616088947024199</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>1.158510638297872</v>
+      </c>
+      <c r="C70" t="n">
+        <v>1089</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.02154255319148936</v>
+      </c>
+      <c r="E70" t="n">
+        <v>20.25</v>
+      </c>
+      <c r="F70" t="n">
+        <v>107</v>
+      </c>
+      <c r="G70" t="s">
+        <v>44</v>
+      </c>
+      <c r="H70" t="s">
+        <v>18</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0.1138297872340426</v>
+      </c>
+      <c r="J70" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="K70" t="n">
+        <v>0.0007978723404255319</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="n">
+        <v>3.703620136892431</v>
+      </c>
+      <c r="C71" t="n">
+        <v>6127.25</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.04150350867466872</v>
+      </c>
+      <c r="E71" t="n">
+        <v>67</v>
+      </c>
+      <c r="F71" t="n">
+        <v>168.5</v>
+      </c>
+      <c r="G71" t="s">
+        <v>45</v>
+      </c>
+      <c r="H71" t="s">
+        <v>18</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0.1027973605081667</v>
+      </c>
+      <c r="J71" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="K71" t="n">
+        <v>0.005183907954944446</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="n">
+        <v>1.933228192857932</v>
+      </c>
+      <c r="C72" t="n">
+        <v>2893.4</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0.02065910352140298</v>
+      </c>
+      <c r="E72" t="n">
+        <v>31.2</v>
+      </c>
+      <c r="F72" t="n">
+        <v>184.8</v>
+      </c>
+      <c r="G72" t="s">
+        <v>43</v>
+      </c>
+      <c r="H72" t="s">
+        <v>18</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0.1252319415552276</v>
+      </c>
+      <c r="J72" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="K72" t="n">
+        <v>0.006262433353588783</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="n">
+        <v>2.278052291732825</v>
+      </c>
+      <c r="C73" t="n">
+        <v>1142.8</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.0271842913094104</v>
+      </c>
+      <c r="E73" t="n">
+        <v>18.2</v>
+      </c>
+      <c r="F73" t="n">
+        <v>122.4</v>
+      </c>
+      <c r="G73" t="s">
+        <v>44</v>
+      </c>
+      <c r="H73" t="s">
+        <v>18</v>
+      </c>
+      <c r="I73" t="n">
+        <v>0.2741484069016619</v>
+      </c>
+      <c r="J73" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="K73" t="n">
+        <v>0.0006382978723404255</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="n">
+        <v>2.962896109513945</v>
+      </c>
+      <c r="C74" t="n">
+        <v>4901.8</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.03320280693973497</v>
+      </c>
+      <c r="E74" t="n">
+        <v>53.6</v>
+      </c>
+      <c r="F74" t="n">
+        <v>134.8</v>
+      </c>
+      <c r="G74" t="s">
+        <v>45</v>
+      </c>
+      <c r="H74" t="s">
+        <v>18</v>
+      </c>
+      <c r="I74" t="n">
+        <v>0.08223788840653333</v>
+      </c>
+      <c r="J74" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="K74" t="n">
+        <v>0.004147126363955557</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="n">
+        <v>6.710934922957702</v>
+      </c>
+      <c r="C75" t="n">
+        <v>11434.2</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.0404788960127518</v>
+      </c>
+      <c r="E75" t="n">
+        <v>62.2</v>
+      </c>
+      <c r="F75" t="n">
+        <v>338.2</v>
+      </c>
+      <c r="G75" t="s">
+        <v>46</v>
+      </c>
+      <c r="H75" t="s">
+        <v>18</v>
+      </c>
+      <c r="I75" t="n">
+        <v>0.2035710766994756</v>
+      </c>
+      <c r="J75" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="K75" t="n">
+        <v>0.004878862988729487</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="n">
+        <v>8.922961909838907</v>
+      </c>
+      <c r="C76" t="n">
+        <v>15499.4</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0.0439786500407446</v>
+      </c>
+      <c r="E76" t="n">
+        <v>78.59999999999999</v>
+      </c>
+      <c r="F76" t="n">
+        <v>418.4</v>
+      </c>
+      <c r="G76" t="s">
+        <v>14</v>
+      </c>
+      <c r="H76" t="s">
+        <v>11</v>
+      </c>
+      <c r="I76" t="n">
+        <v>0.2610849084904173</v>
+      </c>
+      <c r="J76" t="n">
+        <v>18.2</v>
+      </c>
+      <c r="K76" t="n">
+        <v>0.01083898607259163</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="n">
+        <v>7.352278870698461</v>
+      </c>
+      <c r="C77" t="n">
+        <v>13452.8</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0.03998785955724499</v>
+      </c>
+      <c r="E77" t="n">
+        <v>73.40000000000001</v>
+      </c>
+      <c r="F77" t="n">
+        <v>290.2</v>
+      </c>
+      <c r="G77" t="s">
+        <v>14</v>
+      </c>
+      <c r="H77" t="s">
+        <v>11</v>
+      </c>
+      <c r="I77" t="n">
+        <v>0.1626965738779845</v>
+      </c>
+      <c r="J77" t="n">
+        <v>14.6</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0.008076131122476515</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B78" t="n">
+        <v>3.203383214053351</v>
+      </c>
+      <c r="C78" t="n">
+        <v>4923.6</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0.01535458685751464</v>
+      </c>
+      <c r="E78" t="n">
+        <v>23.6</v>
+      </c>
+      <c r="F78" t="n">
+        <v>126</v>
+      </c>
+      <c r="G78" t="s">
+        <v>10</v>
+      </c>
+      <c r="H78" t="s">
+        <v>11</v>
+      </c>
+      <c r="I78" t="n">
+        <v>0.08197787898503578</v>
+      </c>
+      <c r="J78" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="K78" t="n">
+        <v>0.0022121014964216</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B79" t="n">
+        <v>1.775319622012229</v>
+      </c>
+      <c r="C79" t="n">
+        <v>3193.8</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0.01634241245136187</v>
+      </c>
+      <c r="E79" t="n">
+        <v>29.4</v>
+      </c>
+      <c r="F79" t="n">
+        <v>41</v>
+      </c>
+      <c r="G79" t="s">
+        <v>12</v>
+      </c>
+      <c r="H79" t="s">
+        <v>11</v>
+      </c>
+      <c r="I79" t="n">
+        <v>0.02279043913285158</v>
+      </c>
+      <c r="J79" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="K79" t="n">
+        <v>0.002445803224013341</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B80" t="n">
+        <v>4.58653314427508</v>
+      </c>
+      <c r="C80" t="n">
+        <v>8017.8</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.03247285569866215</v>
+      </c>
+      <c r="E80" t="n">
+        <v>56.2</v>
+      </c>
+      <c r="F80" t="n">
+        <v>187.4</v>
+      </c>
+      <c r="G80" t="s">
+        <v>13</v>
+      </c>
+      <c r="H80" t="s">
+        <v>11</v>
+      </c>
+      <c r="I80" t="n">
+        <v>0.1066721808657292</v>
+      </c>
+      <c r="J80" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="K80" t="n">
+        <v>0.003094384707287933</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
+      <c r="A81" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B81" t="n">
         <v>1.901710291787398</v>
       </c>
-      <c r="C58" t="n">
+      <c r="C81" t="n">
         <v>4185.8</v>
       </c>
-      <c r="D58" t="n">
+      <c r="D81" t="n">
         <v>0.01349240180076153</v>
       </c>
-      <c r="E58" t="n">
+      <c r="E81" t="n">
         <v>29.6</v>
       </c>
-      <c r="F58" t="n">
+      <c r="F81" t="n">
         <v>204.4</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G81" t="s">
         <v>15</v>
       </c>
-      <c r="H58" t="s">
+      <c r="H81" t="s">
         <v>16</v>
       </c>
-      <c r="I58" t="n">
+      <c r="I81" t="n">
         <v>0.09128055152368671</v>
       </c>
-      <c r="J58" t="n">
+      <c r="J81" t="n">
         <v>18.6</v>
       </c>
-      <c r="K58" t="n">
+      <c r="K81" t="n">
         <v>0.008167217339014521</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added jquery to index form
</commit_message>
<xml_diff>
--- a/lolMineSite/results/api/lol.xlsx
+++ b/lolMineSite/results/api/lol.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
   <si>
     <t>Aggression Point</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>MagusApex</t>
+  </si>
+  <si>
+    <t>Shiller</t>
   </si>
 </sst>
 </file>
@@ -522,7 +525,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K99"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3846,142 +3849,177 @@
     </row>
     <row r="96" spans="1:11">
       <c r="A96" s="1" t="n">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B96" t="n">
-        <v>3.07100063734863</v>
+        <v>1.901710291787398</v>
       </c>
       <c r="C96" t="n">
-        <v>4818.4</v>
+        <v>4185.8</v>
       </c>
       <c r="D96" t="n">
-        <v>0.02179732313575526</v>
+        <v>0.01349240180076153</v>
       </c>
       <c r="E96" t="n">
-        <v>34.2</v>
+        <v>29.6</v>
       </c>
       <c r="F96" t="n">
-        <v>198</v>
+        <v>204.4</v>
       </c>
       <c r="G96" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="H96" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I96" t="n">
-        <v>0.1261950286806883</v>
+        <v>0.09128055152368671</v>
       </c>
       <c r="J96" t="n">
-        <v>4.8</v>
+        <v>18.6</v>
       </c>
       <c r="K96" t="n">
-        <v>0.003059273422562141</v>
+        <v>0.008167217339014521</v>
       </c>
     </row>
     <row r="97" spans="1:11">
       <c r="A97" s="1" t="n">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B97" t="n">
-        <v>7.829359333360753</v>
+        <v>2.791646791513082</v>
       </c>
       <c r="C97" t="n">
-        <v>16197.8</v>
+        <v>3890.6</v>
       </c>
       <c r="D97" t="n">
-        <v>0.08013202994381621</v>
+        <v>0.01949175076877424</v>
       </c>
       <c r="E97" t="n">
-        <v>165</v>
+        <v>28.2</v>
       </c>
       <c r="F97" t="n">
-        <v>430.2</v>
+        <v>221.4</v>
       </c>
       <c r="G97" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H97" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="I97" t="n">
-        <v>0.2063731471137939</v>
+        <v>0.1749684198889241</v>
       </c>
       <c r="J97" t="n">
-        <v>19.6</v>
+        <v>3.2</v>
       </c>
       <c r="K97" t="n">
-        <v>0.009152606233594018</v>
+        <v>0.002463335941977546</v>
       </c>
     </row>
     <row r="98" spans="1:11">
       <c r="A98" s="1" t="n">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B98" t="n">
-        <v>5.64523200920185</v>
+        <v>2.416763848396501</v>
       </c>
       <c r="C98" t="n">
-        <v>8954.200000000001</v>
+        <v>3315.8</v>
       </c>
       <c r="D98" t="n">
-        <v>0.02991473419815112</v>
+        <v>0.0163265306122449</v>
       </c>
       <c r="E98" t="n">
-        <v>49.4</v>
+        <v>22.4</v>
       </c>
       <c r="F98" t="n">
-        <v>610.2</v>
+        <v>40.6</v>
       </c>
       <c r="G98" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H98" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="I98" t="n">
-        <v>0.3863354585100985</v>
+        <v>0.02959183673469388</v>
       </c>
       <c r="J98" t="n">
-        <v>15.2</v>
+        <v>3.4</v>
       </c>
       <c r="K98" t="n">
-        <v>0.009556019006126104</v>
+        <v>0.002478134110787172</v>
       </c>
     </row>
     <row r="99" spans="1:11">
       <c r="A99" s="1" t="n">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B99" t="n">
-        <v>3.652230980643308</v>
+        <v>9.48417331160671</v>
       </c>
       <c r="C99" t="n">
-        <v>5297.6</v>
+        <v>15096.8</v>
       </c>
       <c r="D99" t="n">
-        <v>0.03020442432290065</v>
+        <v>0.04245232838056302</v>
       </c>
       <c r="E99" t="n">
-        <v>45.8</v>
+        <v>67</v>
       </c>
       <c r="F99" t="n">
-        <v>292</v>
+        <v>161.6</v>
       </c>
       <c r="G99" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H99" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="I99" t="n">
-        <v>0.1968040937674682</v>
+        <v>0.1032920977440951</v>
       </c>
       <c r="J99" t="n">
         <v>5.4</v>
       </c>
       <c r="K99" t="n">
-        <v>0.00344223402841273</v>
+        <v>0.003379839878639451</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
+      <c r="A100" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B100" t="n">
+        <v>1.249264705882353</v>
+      </c>
+      <c r="C100" t="n">
+        <v>2038.8</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0.01409313725490196</v>
+      </c>
+      <c r="E100" t="n">
+        <v>23</v>
+      </c>
+      <c r="F100" t="n">
+        <v>138</v>
+      </c>
+      <c r="G100" t="s">
+        <v>45</v>
+      </c>
+      <c r="H100" t="s">
+        <v>18</v>
+      </c>
+      <c r="I100" t="n">
+        <v>0.08455882352941177</v>
+      </c>
+      <c r="J100" t="n">
+        <v>3</v>
+      </c>
+      <c r="K100" t="n">
+        <v>0.001838235294117647</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
regression and some others
</commit_message>
<xml_diff>
--- a/lolMineSite/results/api/lol.xlsx
+++ b/lolMineSite/results/api/lol.xlsx
@@ -522,7 +522,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K99"/>
+  <dimension ref="A1:K103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3846,90 +3846,92 @@
     </row>
     <row r="96" spans="1:11">
       <c r="A96" s="1" t="n">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>0</v>
+        <v>2.383936531395372</v>
       </c>
       <c r="C96" t="n">
-        <v>0</v>
+        <v>3065.4</v>
       </c>
       <c r="D96" t="n">
-        <v>0</v>
+        <v>0.01186318291444714</v>
       </c>
       <c r="E96" t="n">
-        <v>0</v>
+        <v>14.2</v>
       </c>
       <c r="F96" t="n">
-        <v>0</v>
-      </c>
-      <c r="G96" t="s"/>
+        <v>318.2</v>
+      </c>
+      <c r="G96" t="s">
+        <v>24</v>
+      </c>
       <c r="H96" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I96" t="n">
-        <v>0</v>
+        <v>0.2513900194630072</v>
       </c>
       <c r="J96" t="n">
-        <v>0</v>
+        <v>11.8</v>
       </c>
       <c r="K96" t="n">
-        <v>0</v>
+        <v>0.008399989526632901</v>
       </c>
     </row>
     <row r="97" spans="1:11">
       <c r="A97" s="1" t="n">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B97" t="n">
-        <v>1.775319622012229</v>
+        <v>11.47138019017781</v>
       </c>
       <c r="C97" t="n">
-        <v>3193.8</v>
+        <v>16820.8</v>
       </c>
       <c r="D97" t="n">
-        <v>0.01634241245136187</v>
+        <v>0.1148893923255633</v>
       </c>
       <c r="E97" t="n">
-        <v>29.4</v>
+        <v>165</v>
       </c>
       <c r="F97" t="n">
-        <v>41</v>
+        <v>373.4</v>
       </c>
       <c r="G97" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H97" t="s">
         <v>11</v>
       </c>
       <c r="I97" t="n">
-        <v>0.02279043913285158</v>
+        <v>0.2602785146347409</v>
       </c>
       <c r="J97" t="n">
-        <v>4.4</v>
+        <v>15.4</v>
       </c>
       <c r="K97" t="n">
-        <v>0.002445803224013341</v>
+        <v>0.0102324902907245</v>
       </c>
     </row>
     <row r="98" spans="1:11">
       <c r="A98" s="1" t="n">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B98" t="n">
-        <v>6.474714026753915</v>
+        <v>6.506973090568204</v>
       </c>
       <c r="C98" t="n">
-        <v>8602</v>
+        <v>9534.4</v>
       </c>
       <c r="D98" t="n">
-        <v>0.04634044514716931</v>
+        <v>0.04526183093699399</v>
       </c>
       <c r="E98" t="n">
-        <v>61.2</v>
+        <v>68.8</v>
       </c>
       <c r="F98" t="n">
-        <v>328.6</v>
+        <v>370.2</v>
       </c>
       <c r="G98" t="s">
         <v>14</v>
@@ -3938,47 +3940,185 @@
         <v>11</v>
       </c>
       <c r="I98" t="n">
-        <v>0.2473481266503256</v>
+        <v>0.2520432498535652</v>
       </c>
       <c r="J98" t="n">
-        <v>9.6</v>
+        <v>12.8</v>
       </c>
       <c r="K98" t="n">
-        <v>0.007220967752454279</v>
+        <v>0.008581153657621576</v>
       </c>
     </row>
     <row r="99" spans="1:11">
       <c r="A99" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B99" t="n">
+        <v>0</v>
+      </c>
+      <c r="C99" t="n">
+        <v>0</v>
+      </c>
+      <c r="D99" t="n">
+        <v>0</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0</v>
+      </c>
+      <c r="G99" t="s"/>
+      <c r="H99" t="s">
+        <v>11</v>
+      </c>
+      <c r="I99" t="n">
+        <v>0</v>
+      </c>
+      <c r="J99" t="n">
+        <v>0</v>
+      </c>
+      <c r="K99" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
+      <c r="A100" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B100" t="n">
+        <v>1.775319622012229</v>
+      </c>
+      <c r="C100" t="n">
+        <v>3193.8</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0.01634241245136187</v>
+      </c>
+      <c r="E100" t="n">
+        <v>29.4</v>
+      </c>
+      <c r="F100" t="n">
+        <v>41</v>
+      </c>
+      <c r="G100" t="s">
+        <v>12</v>
+      </c>
+      <c r="H100" t="s">
+        <v>11</v>
+      </c>
+      <c r="I100" t="n">
+        <v>0.02279043913285158</v>
+      </c>
+      <c r="J100" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="K100" t="n">
+        <v>0.002445803224013341</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
+      <c r="A101" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="B99" t="n">
+      <c r="B101" t="n">
+        <v>11.47138019017781</v>
+      </c>
+      <c r="C101" t="n">
+        <v>16820.8</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0.1148893923255633</v>
+      </c>
+      <c r="E101" t="n">
+        <v>165</v>
+      </c>
+      <c r="F101" t="n">
+        <v>373.4</v>
+      </c>
+      <c r="G101" t="s">
+        <v>13</v>
+      </c>
+      <c r="H101" t="s">
+        <v>11</v>
+      </c>
+      <c r="I101" t="n">
+        <v>0.2602785146347409</v>
+      </c>
+      <c r="J101" t="n">
+        <v>15.4</v>
+      </c>
+      <c r="K101" t="n">
+        <v>0.0102324902907245</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
+      <c r="A102" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B102" t="n">
+        <v>6.506973090568204</v>
+      </c>
+      <c r="C102" t="n">
+        <v>9534.4</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0.04526183093699399</v>
+      </c>
+      <c r="E102" t="n">
+        <v>68.8</v>
+      </c>
+      <c r="F102" t="n">
+        <v>370.2</v>
+      </c>
+      <c r="G102" t="s">
+        <v>14</v>
+      </c>
+      <c r="H102" t="s">
+        <v>11</v>
+      </c>
+      <c r="I102" t="n">
+        <v>0.2520432498535652</v>
+      </c>
+      <c r="J102" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="K102" t="n">
+        <v>0.008581153657621576</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
+      <c r="A103" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B103" t="n">
         <v>2.383936531395372</v>
       </c>
-      <c r="C99" t="n">
+      <c r="C103" t="n">
         <v>3065.4</v>
       </c>
-      <c r="D99" t="n">
+      <c r="D103" t="n">
         <v>0.01186318291444714</v>
       </c>
-      <c r="E99" t="n">
+      <c r="E103" t="n">
         <v>14.2</v>
       </c>
-      <c r="F99" t="n">
+      <c r="F103" t="n">
         <v>318.2</v>
       </c>
-      <c r="G99" t="s">
+      <c r="G103" t="s">
         <v>24</v>
       </c>
-      <c r="H99" t="s">
+      <c r="H103" t="s">
         <v>25</v>
       </c>
-      <c r="I99" t="n">
+      <c r="I103" t="n">
         <v>0.2513900194630072</v>
       </c>
-      <c r="J99" t="n">
+      <c r="J103" t="n">
         <v>11.8</v>
       </c>
-      <c r="K99" t="n">
+      <c r="K103" t="n">
         <v>0.008399989526632901</v>
       </c>
     </row>

</xml_diff>

<commit_message>
almost all parts are working but they need maintance
</commit_message>
<xml_diff>
--- a/lolMineSite/results/api/lol.xlsx
+++ b/lolMineSite/results/api/lol.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
   <si>
     <t>Aggression Point</t>
   </si>
@@ -201,6 +201,36 @@
   </si>
   <si>
     <t>Shiller</t>
+  </si>
+  <si>
+    <t>Hakan Muhafız</t>
+  </si>
+  <si>
+    <t>TWİSTED</t>
+  </si>
+  <si>
+    <t>Inmate 4859</t>
+  </si>
+  <si>
+    <t>annemkızıyo</t>
+  </si>
+  <si>
+    <t>BÜYÜK  ÇÜK LAMAR</t>
+  </si>
+  <si>
+    <t>Inuwâ Dân X</t>
+  </si>
+  <si>
+    <t>Takizawà</t>
+  </si>
+  <si>
+    <t>1against9 L9</t>
+  </si>
+  <si>
+    <t>Mr F Scofield</t>
+  </si>
+  <si>
+    <t>atkı</t>
   </si>
 </sst>
 </file>
@@ -549,7 +579,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q121"/>
+  <dimension ref="A1:Q126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5371,7 +5401,7 @@
     </row>
     <row r="114" spans="1:17">
       <c r="A114" s="1" t="n">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B114" t="n">
         <v>2.416763848396501</v>
@@ -5424,7 +5454,7 @@
     </row>
     <row r="115" spans="1:17">
       <c r="A115" s="1" t="n">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B115" t="n">
         <v>7.526515336917045</v>
@@ -5477,7 +5507,7 @@
     </row>
     <row r="116" spans="1:17">
       <c r="A116" s="1" t="n">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B116" t="n">
         <v>1.249264705882353</v>
@@ -5530,267 +5560,532 @@
     </row>
     <row r="117" spans="1:17">
       <c r="A117" s="1" t="n">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>1.901710291787398</v>
+        <v>2.416463478170262</v>
       </c>
       <c r="C117" t="n">
-        <v>4185.8</v>
+        <v>2964.4</v>
       </c>
       <c r="D117" t="n">
-        <v>0.01349240180076153</v>
+        <v>0.03885207398533574</v>
       </c>
       <c r="E117" t="n">
-        <v>29.6</v>
+        <v>48.2</v>
       </c>
       <c r="F117" t="n">
-        <v>204.4</v>
+        <v>171.8</v>
       </c>
       <c r="G117" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="H117" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I117" t="n">
-        <v>0.09128055152368671</v>
+        <v>0.1353850873429003</v>
       </c>
       <c r="J117" t="n">
-        <v>18.6</v>
+        <v>4.6</v>
       </c>
       <c r="K117" t="n">
-        <v>0.008167217339014521</v>
+        <v>0.003765798965385793</v>
       </c>
       <c r="L117" t="n">
-        <v>4.2</v>
+        <v>0.8</v>
       </c>
       <c r="M117" t="n">
-        <v>4</v>
+        <v>1.4</v>
       </c>
       <c r="N117" t="n">
-        <v>2.2</v>
+        <v>1</v>
       </c>
       <c r="O117" t="n">
-        <v>6</v>
+        <v>4.6</v>
       </c>
       <c r="P117" t="n">
-        <v>4185.8</v>
+        <v>2964.4</v>
       </c>
       <c r="Q117" t="n">
-        <v>18.6</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="118" spans="1:17">
       <c r="A118" s="1" t="n">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>2.791646791513082</v>
+        <v>5.161185769562334</v>
       </c>
       <c r="C118" t="n">
-        <v>3890.6</v>
+        <v>8200.6</v>
       </c>
       <c r="D118" t="n">
-        <v>0.01949175076877424</v>
+        <v>0.02945888127014684</v>
       </c>
       <c r="E118" t="n">
-        <v>28.2</v>
+        <v>47.4</v>
       </c>
       <c r="F118" t="n">
         <v>221.4</v>
       </c>
       <c r="G118" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="H118" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I118" t="n">
-        <v>0.1749684198889241</v>
+        <v>0.1383712522209088</v>
       </c>
       <c r="J118" t="n">
-        <v>3.2</v>
+        <v>12.6</v>
       </c>
       <c r="K118" t="n">
-        <v>0.002463335941977546</v>
+        <v>0.008441246441123099</v>
       </c>
       <c r="L118" t="n">
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="M118" t="n">
-        <v>2.2</v>
+        <v>5.2</v>
       </c>
       <c r="N118" t="n">
-        <v>1.8</v>
+        <v>1.6</v>
       </c>
       <c r="O118" t="n">
-        <v>5.6</v>
+        <v>14.6</v>
       </c>
       <c r="P118" t="n">
-        <v>3890.6</v>
+        <v>8200.6</v>
       </c>
       <c r="Q118" t="n">
-        <v>3.2</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="119" spans="1:17">
       <c r="A119" s="1" t="n">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>2.416763848396501</v>
+        <v>2.068847369766977</v>
       </c>
       <c r="C119" t="n">
-        <v>3315.8</v>
+        <v>3795.4</v>
       </c>
       <c r="D119" t="n">
-        <v>0.0163265306122449</v>
+        <v>0.005055885542121584</v>
       </c>
       <c r="E119" t="n">
-        <v>22.4</v>
+        <v>10</v>
       </c>
       <c r="F119" t="n">
-        <v>40.6</v>
+        <v>241.4</v>
       </c>
       <c r="G119" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="H119" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="I119" t="n">
-        <v>0.02959183673469388</v>
+        <v>0.1233551760989223</v>
       </c>
       <c r="J119" t="n">
-        <v>3.4</v>
+        <v>12</v>
       </c>
       <c r="K119" t="n">
-        <v>0.002478134110787172</v>
+        <v>0.005858238664598527</v>
       </c>
       <c r="L119" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="M119" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="N119" t="n">
         <v>1.8</v>
       </c>
-      <c r="M119" t="n">
-        <v>2</v>
-      </c>
-      <c r="N119" t="n">
-        <v>0.6</v>
-      </c>
       <c r="O119" t="n">
-        <v>3.8</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="P119" t="n">
-        <v>3315.8</v>
+        <v>3795.4</v>
       </c>
       <c r="Q119" t="n">
-        <v>3.4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="120" spans="1:17">
       <c r="A120" s="1" t="n">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>7.526515336917045</v>
+        <v>1.505994397759104</v>
       </c>
       <c r="C120" t="n">
-        <v>12752.4</v>
+        <v>2688.2</v>
       </c>
       <c r="D120" t="n">
-        <v>0.04081966133960498</v>
+        <v>0.01490196078431373</v>
       </c>
       <c r="E120" t="n">
-        <v>72.8</v>
+        <v>26.6</v>
       </c>
       <c r="F120" t="n">
-        <v>209.8</v>
+        <v>45.6</v>
       </c>
       <c r="G120" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H120" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="I120" t="n">
-        <v>0.1137729726188463</v>
+        <v>0.02554621848739496</v>
       </c>
       <c r="J120" t="n">
-        <v>7</v>
+        <v>2.8</v>
       </c>
       <c r="K120" t="n">
-        <v>0.003974587084214064</v>
+        <v>0.001568627450980392</v>
       </c>
       <c r="L120" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M120" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="N120" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="O120" t="n">
         <v>2.4</v>
       </c>
-      <c r="N120" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="O120" t="n">
-        <v>1.4</v>
-      </c>
       <c r="P120" t="n">
-        <v>12752.4</v>
+        <v>2688.2</v>
       </c>
       <c r="Q120" t="n">
-        <v>7</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="121" spans="1:17">
       <c r="A121" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B121" t="n">
+        <v>3.799488925521617</v>
+      </c>
+      <c r="C121" t="n">
+        <v>7293.8</v>
+      </c>
+      <c r="D121" t="n">
+        <v>0.01015607778491264</v>
+      </c>
+      <c r="E121" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="F121" t="n">
+        <v>275.4</v>
+      </c>
+      <c r="G121" t="s">
+        <v>66</v>
+      </c>
+      <c r="H121" t="s">
+        <v>31</v>
+      </c>
+      <c r="I121" t="n">
+        <v>0.1551790318097739</v>
+      </c>
+      <c r="J121" t="n">
+        <v>6</v>
+      </c>
+      <c r="K121" t="n">
+        <v>0.003255853515943223</v>
+      </c>
+      <c r="L121" t="n">
+        <v>3</v>
+      </c>
+      <c r="M121" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="N121" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="O121" t="n">
+        <v>13.6</v>
+      </c>
+      <c r="P121" t="n">
+        <v>7293.8</v>
+      </c>
+      <c r="Q121" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:17">
+      <c r="A122" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" t="n">
+        <v>5.552368248186704</v>
+      </c>
+      <c r="C122" t="n">
+        <v>13156.8</v>
+      </c>
+      <c r="D122" t="n">
+        <v>0.03811254470716262</v>
+      </c>
+      <c r="E122" t="n">
+        <v>92.2</v>
+      </c>
+      <c r="F122" t="n">
+        <v>208.8</v>
+      </c>
+      <c r="G122" t="s">
+        <v>67</v>
+      </c>
+      <c r="H122" t="s">
+        <v>33</v>
+      </c>
+      <c r="I122" t="n">
+        <v>0.08970024567781631</v>
+      </c>
+      <c r="J122" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="K122" t="n">
+        <v>0.0041437734423764</v>
+      </c>
+      <c r="L122" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="M122" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="N122" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="O122" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="P122" t="n">
+        <v>13156.8</v>
+      </c>
+      <c r="Q122" t="n">
+        <v>10.2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17">
+      <c r="A123" s="1" t="n">
         <v>121</v>
       </c>
-      <c r="B121" t="n">
-        <v>1.249264705882353</v>
-      </c>
-      <c r="C121" t="n">
-        <v>2038.8</v>
-      </c>
-      <c r="D121" t="n">
-        <v>0.01409313725490196</v>
-      </c>
-      <c r="E121" t="n">
-        <v>23</v>
-      </c>
-      <c r="F121" t="n">
-        <v>138</v>
-      </c>
-      <c r="G121" t="s">
-        <v>51</v>
-      </c>
-      <c r="H121" t="s">
+      <c r="B123" t="n">
+        <v>8.640537996803857</v>
+      </c>
+      <c r="C123" t="n">
+        <v>19508.6</v>
+      </c>
+      <c r="D123" t="n">
+        <v>0.06836728990692152</v>
+      </c>
+      <c r="E123" t="n">
+        <v>110.8</v>
+      </c>
+      <c r="F123" t="n">
+        <v>342.8</v>
+      </c>
+      <c r="G123" t="s">
+        <v>68</v>
+      </c>
+      <c r="H123" t="s">
         <v>24</v>
       </c>
-      <c r="I121" t="n">
-        <v>0.08455882352941177</v>
-      </c>
-      <c r="J121" t="n">
-        <v>3</v>
-      </c>
-      <c r="K121" t="n">
-        <v>0.001838235294117647</v>
-      </c>
-      <c r="L121" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="M121" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="N121" t="n">
+      <c r="I123" t="n">
+        <v>0.1609056249067745</v>
+      </c>
+      <c r="J123" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="K123" t="n">
+        <v>0.008901090469941059</v>
+      </c>
+      <c r="L123" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="M123" t="n">
+        <v>4</v>
+      </c>
+      <c r="N123" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="O123" t="n">
+        <v>14</v>
+      </c>
+      <c r="P123" t="n">
+        <v>19508.6</v>
+      </c>
+      <c r="Q123" t="n">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:17">
+      <c r="A124" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="B124" t="n">
+        <v>4.958948577935138</v>
+      </c>
+      <c r="C124" t="n">
+        <v>7422.2</v>
+      </c>
+      <c r="D124" t="n">
+        <v>0.05297472115560431</v>
+      </c>
+      <c r="E124" t="n">
+        <v>75.8</v>
+      </c>
+      <c r="F124" t="n">
+        <v>343.6</v>
+      </c>
+      <c r="G124" t="s">
+        <v>69</v>
+      </c>
+      <c r="H124" t="s">
+        <v>24</v>
+      </c>
+      <c r="I124" t="n">
+        <v>0.2438613715321066</v>
+      </c>
+      <c r="J124" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="K124" t="n">
+        <v>0.003429869180006317</v>
+      </c>
+      <c r="L124" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="M124" t="n">
         <v>1.2</v>
       </c>
-      <c r="O121" t="n">
-        <v>2</v>
-      </c>
-      <c r="P121" t="n">
-        <v>2038.8</v>
-      </c>
-      <c r="Q121" t="n">
-        <v>3</v>
+      <c r="N124" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="O124" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="P124" t="n">
+        <v>7422.2</v>
+      </c>
+      <c r="Q124" t="n">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17">
+      <c r="A125" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="B125" t="n">
+        <v>7.578175204713018</v>
+      </c>
+      <c r="C125" t="n">
+        <v>13639.6</v>
+      </c>
+      <c r="D125" t="n">
+        <v>0.07927726354393795</v>
+      </c>
+      <c r="E125" t="n">
+        <v>145</v>
+      </c>
+      <c r="F125" t="n">
+        <v>588.4</v>
+      </c>
+      <c r="G125" t="s">
+        <v>70</v>
+      </c>
+      <c r="H125" t="s">
+        <v>24</v>
+      </c>
+      <c r="I125" t="n">
+        <v>0.3224582848240293</v>
+      </c>
+      <c r="J125" t="n">
+        <v>12</v>
+      </c>
+      <c r="K125" t="n">
+        <v>0.006465115763260081</v>
+      </c>
+      <c r="L125" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="M125" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="N125" t="n">
+        <v>6</v>
+      </c>
+      <c r="O125" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="P125" t="n">
+        <v>13639.6</v>
+      </c>
+      <c r="Q125" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17">
+      <c r="A126" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="B126" t="n">
+        <v>4.718499124373624</v>
+      </c>
+      <c r="C126" t="n">
+        <v>6698</v>
+      </c>
+      <c r="D126" t="n">
+        <v>0.03749183615672267</v>
+      </c>
+      <c r="E126" t="n">
+        <v>52.4</v>
+      </c>
+      <c r="F126" t="n">
+        <v>260.8</v>
+      </c>
+      <c r="G126" t="s">
+        <v>71</v>
+      </c>
+      <c r="H126" t="s">
+        <v>24</v>
+      </c>
+      <c r="I126" t="n">
+        <v>0.19180321236396</v>
+      </c>
+      <c r="J126" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="K126" t="n">
+        <v>0.005053780220669405</v>
+      </c>
+      <c r="L126" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="M126" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="N126" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="O126" t="n">
+        <v>11.4</v>
+      </c>
+      <c r="P126" t="n">
+        <v>6698</v>
+      </c>
+      <c r="Q126" t="n">
+        <v>7.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>